<commit_message>
Finish own todo list
</commit_message>
<xml_diff>
--- a/ITU/todolist.xlsx
+++ b/ITU/todolist.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="SETUP" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Estimation" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="TODO" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="General" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="SETUP" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,31 +23,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">qui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somme de estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mickael</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yvan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanekena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">module/fonctionnalité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temps passé </t>
+  </si>
+  <si>
+    <t xml:space="preserve">reste à faire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avancement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Authentification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage</t>
+  </si>
   <si>
     <t xml:space="preserve">module/fonctionnalité </t>
   </si>
   <si>
-    <t xml:space="preserve">page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
     <t xml:space="preserve">qui </t>
   </si>
   <si>
-    <t xml:space="preserve">Affichage</t>
+    <t xml:space="preserve">Landing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +125,36 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.5999"/>
+        <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -85,8 +162,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -110,28 +250,112 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="24" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Pivot Table Field" xfId="20"/>
+    <cellStyle name="Pivot Table Category" xfId="21"/>
+    <cellStyle name="Pivot Table Title" xfId="22"/>
+    <cellStyle name="Pivot Table Corner" xfId="23"/>
+    <cellStyle name="Pivot Table Value" xfId="24"/>
+    <cellStyle name="Pivot Table Result" xfId="25"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -150,11 +374,95 @@
       </fill>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFE699"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="type" displayName="type" ref="F5:F6" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="module" displayName="module" ref="B6:B30" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Authentification"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="page" displayName="page" ref="D6:D30" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Landing"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="qui" displayName="qui" ref="H6:H8" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="1">
+    <tableColumn id="1" name="Mickael"/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="type" displayName="type" ref="F5:F9" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="1">
     <tableColumn id="1" name="type"/>
   </tableColumns>
@@ -338,48 +646,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B5:H6"/>
+  <dimension ref="A3:B10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.53"/>
   </cols>
   <sheetData>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="B4" s="4" t="n">
+        <f aca="false">SUMIF(TODO!E:E, "Mickael", TODO!F:F)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="0" t="s">
+      <c r="B5" s="6" t="n">
+        <f aca="false">SUMIF(TODO!E:E, "Yvan", TODO!F:F)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
+      <c r="B6" s="7" t="n">
+        <f aca="false">SUMIF(TODO!E:E, "Fanekena", TODO!F:F)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="n">
+        <f aca="false">SUM(B4:B6)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
-  <tableParts>
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -388,82 +719,712 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="E1:E20"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="10" width="11.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E1" s="0" t="s">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="2" t="s">
-        <v>4</v>
+      <c r="F2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">F2-G2</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="14" t="n">
+        <f aca="false">G2/(G2+H2)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="2"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="2"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="2"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="2"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="2"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="2"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="2"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="2"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E11" s="2"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="2"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="E12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="2"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="E13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="2"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E15" s="2"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="2"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E17" s="2"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="E17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="2"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="E18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E19" s="2"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="E19" s="15"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="2"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="E27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="E28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="E30" s="13"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="E31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="E32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="E33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="E34" s="13"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="E35" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="E37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="E38" s="13"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="E41" s="13"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="E42" s="13"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="E43" s="13"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="E44" s="13"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="E45" s="13"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="E46" s="13"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="E47" s="13"/>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="E48" s="13"/>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="E49" s="13"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="E50" s="13"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="E51" s="13"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="E53" s="13"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="E55" s="13"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="E56" s="13"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="E58" s="13"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="E59" s="13"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="E60" s="13"/>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="E61" s="13"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="E62" s="13"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="E63" s="13"/>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="E64" s="13"/>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="E65" s="13"/>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="E67" s="13"/>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="E69" s="13"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="E70" s="13"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="E72" s="13"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="E73" s="13"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="E74" s="13"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="E75" s="13"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="E78" s="13"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="E79" s="13"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="13"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="E80" s="13"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="E81" s="13"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="E82" s="13"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="E83" s="13"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="E84" s="13"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="E85" s="13"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="13"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="E86" s="13"/>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="13"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="E87" s="13"/>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="E88" s="13"/>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="E89" s="13"/>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="13"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="E90" s="13"/>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="E91" s="13"/>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="E92" s="13"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="E93" s="13"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="13"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="E94" s="13"/>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="13"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+      <c r="E95" s="13"/>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="E96" s="13"/>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="13"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="E97" s="13"/>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="E98" s="13"/>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="13"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="E99" s="13"/>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="E100" s="13"/>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E101" s="13"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E102" s="13"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E103" s="13"/>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E104" s="13"/>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E105" s="13"/>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E106" s="13"/>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E107" s="13"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E108" s="13"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E109" s="13"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E110" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E20" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C100" type="list">
       <formula1>type</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E110" type="list">
+      <formula1>qui</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B100" type="list">
+      <formula1>page</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A100" type="list">
+      <formula1>module</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -475,4 +1436,146 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <f aca="false">SUM(TODO!F2:F1001)</f>
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">SUM(TODO!G2:G1001)</f>
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">SUM(TODO!H2:H1001)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <f aca="false">B2/(B2+C2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B5:H9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="16" width="4.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="19.08"/>
+  </cols>
+  <sheetData>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>